<commit_message>
evaporation properties do not get tracked
</commit_message>
<xml_diff>
--- a/tests/data/tfsc_test_experiment.xlsx
+++ b/tests/data/tfsc_test_experiment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="187">
   <si>
     <t xml:space="preserve">Experiment Info</t>
   </si>
@@ -289,6 +289,24 @@
     <t xml:space="preserve">Annealing atmosphere</t>
   </si>
   <si>
+    <t xml:space="preserve">Flow rate [ul/min]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head gap [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air knife angle [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air knife gap [cm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bead volume [mm/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drying speed [cm/min]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gas</t>
   </si>
   <si>
@@ -314,33 +332,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nozzle size [mm²]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vacuum quenching start time [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vacuum quenching duration [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vacuum quenching pressure [bar]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flow rate [ul/min]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Head gap [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air knife angle [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air knife gap [cm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bead volume [mm/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drying speed [cm/min]</t>
   </si>
   <si>
     <t xml:space="preserve">Printhead name</t>
@@ -1131,10 +1122,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IP3"/>
+  <dimension ref="A1:IA3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="FL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="GA2" activeCellId="0" sqref="GA2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1218,165 +1209,151 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="87" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="102" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="109" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="111" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="113" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="116" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="118" min="117" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="119" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="120" min="120" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="121" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="123" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="124" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="126" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="129" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="131" min="131" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="132" min="132" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="133" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="135" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="136" min="136" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="137" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="138" min="138" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="139" min="139" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="140" min="140" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="141" min="141" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="143" min="143" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="144" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="146" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="90" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="105" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="109" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="111" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="113" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="116" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="118" min="117" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="119" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="120" min="120" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="121" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="123" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="124" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="126" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="0" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="129" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="131" min="131" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="132" min="132" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="133" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="135" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="136" min="136" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="137" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="138" min="138" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="139" min="139" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="140" min="140" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="141" min="141" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="143" min="143" style="0" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="144" min="144" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="145" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="146" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="147" min="147" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="148" min="148" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="149" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="150" min="150" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="148" min="148" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="149" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="150" min="150" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="151" min="151" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="152" min="152" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="153" min="153" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="154" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="155" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="156" min="156" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="157" min="157" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="158" min="158" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="159" min="159" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="160" min="160" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="161" min="161" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="162" min="162" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="163" min="163" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="164" min="164" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="165" min="165" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="166" min="166" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="167" min="167" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="168" min="168" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="169" min="169" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="170" min="170" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="152" min="152" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="153" min="153" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="154" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="155" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="156" min="156" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="157" min="157" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="158" min="158" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="160" min="159" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="161" min="161" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="162" min="162" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="163" min="163" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="165" min="164" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="166" min="166" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="167" min="167" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="168" min="168" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="170" min="169" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="171" min="171" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="172" min="172" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="173" min="173" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="175" min="174" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="176" min="176" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="177" min="177" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="178" min="178" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="180" min="179" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="181" min="181" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="182" min="182" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="183" min="183" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="184" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="186" min="186" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="187" min="187" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="188" min="188" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="189" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="172" min="172" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="173" min="173" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="174" min="174" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="175" min="175" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="176" min="176" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="177" min="177" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="178" min="178" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="179" min="179" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="180" min="180" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="181" min="181" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="183" min="182" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="184" min="184" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="185" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="186" min="186" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="187" min="187" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="188" min="188" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="189" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="190" min="190" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="191" min="191" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="192" min="192" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="193" min="193" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="195" min="195" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="196" min="196" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="197" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="199" min="199" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="200" min="200" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="201" min="201" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="202" min="202" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="191" min="191" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="192" min="192" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="193" min="193" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="195" min="195" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="196" min="196" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="197" min="197" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="198" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="199" min="199" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="200" min="200" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="201" min="201" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="202" min="202" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="203" min="203" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="204" min="204" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="205" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="206" min="206" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="207" min="207" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="208" min="208" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="209" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="210" min="210" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="211" min="211" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="212" min="212" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="213" min="213" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="215" min="215" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="216" min="216" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="217" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="219" min="219" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="220" min="220" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="221" min="221" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="222" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="204" min="204" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="205" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="206" min="206" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="207" min="207" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="208" min="208" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="209" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="210" min="210" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="211" min="211" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="212" min="212" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="213" min="213" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="215" min="215" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="216" min="216" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="217" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="219" min="219" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="220" min="220" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="221" min="221" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="222" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="223" min="223" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="224" min="224" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="225" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="226" min="226" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="227" min="227" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="228" min="228" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="229" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="230" min="230" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="231" min="231" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="232" min="232" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="233" min="233" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="235" min="235" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="236" min="236" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="237" min="237" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="238" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="239" min="239" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="240" min="240" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="241" min="241" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="242" min="242" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="243" min="243" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="244" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="245" min="245" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="246" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="247" min="247" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="248" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="249" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="250" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="224" min="224" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="225" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="226" min="226" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="227" min="227" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="228" min="228" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="229" style="0" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="230" min="230" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="231" min="231" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="232" min="232" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="233" min="233" style="0" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="235" min="235" style="0" width="32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,21 +1451,21 @@
       <c r="CB1" s="6"/>
       <c r="CC1" s="6"/>
       <c r="CD1" s="6"/>
-      <c r="CE1" s="6"/>
-      <c r="CF1" s="6"/>
-      <c r="CG1" s="6"/>
-      <c r="CH1" s="6"/>
-      <c r="CI1" s="6"/>
-      <c r="CJ1" s="6"/>
-      <c r="CK1" s="6"/>
-      <c r="CL1" s="6"/>
-      <c r="CM1" s="6"/>
-      <c r="CN1" s="6"/>
-      <c r="CO1" s="6"/>
-      <c r="CP1" s="6"/>
-      <c r="CQ1" s="7" t="s">
+      <c r="CE1" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="CF1" s="7"/>
+      <c r="CG1" s="7"/>
+      <c r="CH1" s="7"/>
+      <c r="CI1" s="7"/>
+      <c r="CJ1" s="7"/>
+      <c r="CK1" s="7"/>
+      <c r="CL1" s="7"/>
+      <c r="CM1" s="7"/>
+      <c r="CN1" s="7"/>
+      <c r="CO1" s="7"/>
+      <c r="CP1" s="7"/>
+      <c r="CQ1" s="7"/>
       <c r="CR1" s="7"/>
       <c r="CS1" s="7"/>
       <c r="CT1" s="7"/>
@@ -1515,24 +1492,24 @@
       <c r="DO1" s="7"/>
       <c r="DP1" s="7"/>
       <c r="DQ1" s="7"/>
-      <c r="DR1" s="7"/>
-      <c r="DS1" s="7"/>
-      <c r="DT1" s="7"/>
-      <c r="DU1" s="7"/>
-      <c r="DV1" s="7"/>
-      <c r="DW1" s="7"/>
-      <c r="DX1" s="7"/>
-      <c r="DY1" s="7"/>
-      <c r="DZ1" s="7"/>
-      <c r="EA1" s="7"/>
-      <c r="EB1" s="7"/>
-      <c r="EC1" s="7"/>
-      <c r="ED1" s="7"/>
-      <c r="EE1" s="7"/>
-      <c r="EF1" s="7"/>
-      <c r="EG1" s="8" t="s">
+      <c r="DR1" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="DS1" s="8"/>
+      <c r="DT1" s="8"/>
+      <c r="DU1" s="8"/>
+      <c r="DV1" s="8"/>
+      <c r="DW1" s="8"/>
+      <c r="DX1" s="8"/>
+      <c r="DY1" s="8"/>
+      <c r="DZ1" s="8"/>
+      <c r="EA1" s="8"/>
+      <c r="EB1" s="8"/>
+      <c r="EC1" s="8"/>
+      <c r="ED1" s="8"/>
+      <c r="EE1" s="8"/>
+      <c r="EF1" s="8"/>
+      <c r="EG1" s="8"/>
       <c r="EH1" s="8"/>
       <c r="EI1" s="8"/>
       <c r="EJ1" s="8"/>
@@ -1540,24 +1517,24 @@
       <c r="EL1" s="8"/>
       <c r="EM1" s="8"/>
       <c r="EN1" s="8"/>
-      <c r="EO1" s="8"/>
-      <c r="EP1" s="8"/>
-      <c r="EQ1" s="8"/>
-      <c r="ER1" s="8"/>
-      <c r="ES1" s="8"/>
-      <c r="ET1" s="8"/>
-      <c r="EU1" s="8"/>
-      <c r="EV1" s="8"/>
-      <c r="EW1" s="8"/>
-      <c r="EX1" s="8"/>
-      <c r="EY1" s="8"/>
-      <c r="EZ1" s="8"/>
-      <c r="FA1" s="8"/>
-      <c r="FB1" s="8"/>
-      <c r="FC1" s="8"/>
-      <c r="FD1" s="9" t="s">
+      <c r="EO1" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="EP1" s="9"/>
+      <c r="EQ1" s="9"/>
+      <c r="ER1" s="9"/>
+      <c r="ES1" s="9"/>
+      <c r="ET1" s="9"/>
+      <c r="EU1" s="9"/>
+      <c r="EV1" s="9"/>
+      <c r="EW1" s="9"/>
+      <c r="EX1" s="9"/>
+      <c r="EY1" s="9"/>
+      <c r="EZ1" s="9"/>
+      <c r="FA1" s="9"/>
+      <c r="FB1" s="9"/>
+      <c r="FC1" s="9"/>
+      <c r="FD1" s="9"/>
       <c r="FE1" s="9"/>
       <c r="FF1" s="9"/>
       <c r="FG1" s="9"/>
@@ -1566,98 +1543,83 @@
       <c r="FJ1" s="9"/>
       <c r="FK1" s="9"/>
       <c r="FL1" s="9"/>
-      <c r="FM1" s="9"/>
-      <c r="FN1" s="9"/>
-      <c r="FO1" s="9"/>
-      <c r="FP1" s="9"/>
-      <c r="FQ1" s="9"/>
-      <c r="FR1" s="9"/>
-      <c r="FS1" s="9"/>
-      <c r="FT1" s="9"/>
-      <c r="FU1" s="9"/>
-      <c r="FV1" s="9"/>
-      <c r="FW1" s="9"/>
-      <c r="FX1" s="9"/>
-      <c r="FY1" s="9"/>
-      <c r="FZ1" s="9"/>
-      <c r="GA1" s="9"/>
-      <c r="GB1" s="10" t="s">
+      <c r="FM1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="GC1" s="10"/>
-      <c r="GD1" s="10"/>
-      <c r="GE1" s="10"/>
-      <c r="GF1" s="10"/>
-      <c r="GG1" s="10"/>
-      <c r="GH1" s="10"/>
-      <c r="GI1" s="10"/>
-      <c r="GJ1" s="10"/>
-      <c r="GK1" s="10"/>
-      <c r="GL1" s="10"/>
-      <c r="GM1" s="10"/>
-      <c r="GN1" s="10"/>
-      <c r="GO1" s="1" t="s">
+      <c r="FN1" s="10"/>
+      <c r="FO1" s="10"/>
+      <c r="FP1" s="10"/>
+      <c r="FQ1" s="10"/>
+      <c r="FR1" s="10"/>
+      <c r="FS1" s="10"/>
+      <c r="FT1" s="10"/>
+      <c r="FU1" s="10"/>
+      <c r="FV1" s="10"/>
+      <c r="FW1" s="10"/>
+      <c r="FX1" s="10"/>
+      <c r="FY1" s="10"/>
+      <c r="FZ1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="GP1" s="1"/>
-      <c r="GQ1" s="1"/>
-      <c r="GR1" s="1"/>
-      <c r="GS1" s="1"/>
-      <c r="GT1" s="1"/>
-      <c r="GU1" s="1"/>
-      <c r="GV1" s="1"/>
-      <c r="GW1" s="1"/>
-      <c r="GX1" s="1"/>
-      <c r="GY1" s="1"/>
-      <c r="GZ1" s="1"/>
-      <c r="HA1" s="1"/>
-      <c r="HB1" s="2" t="s">
+      <c r="GA1" s="1"/>
+      <c r="GB1" s="1"/>
+      <c r="GC1" s="1"/>
+      <c r="GD1" s="1"/>
+      <c r="GE1" s="1"/>
+      <c r="GF1" s="1"/>
+      <c r="GG1" s="1"/>
+      <c r="GH1" s="1"/>
+      <c r="GI1" s="1"/>
+      <c r="GJ1" s="1"/>
+      <c r="GK1" s="1"/>
+      <c r="GL1" s="1"/>
+      <c r="GM1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="GN1" s="2"/>
+      <c r="GO1" s="2"/>
+      <c r="GP1" s="2"/>
+      <c r="GQ1" s="2"/>
+      <c r="GR1" s="2"/>
+      <c r="GS1" s="2"/>
+      <c r="GT1" s="2"/>
+      <c r="GU1" s="2"/>
+      <c r="GV1" s="2"/>
+      <c r="GW1" s="2"/>
+      <c r="GX1" s="2"/>
+      <c r="GY1" s="2"/>
+      <c r="GZ1" s="2"/>
+      <c r="HA1" s="2"/>
+      <c r="HB1" s="2"/>
       <c r="HC1" s="2"/>
       <c r="HD1" s="2"/>
-      <c r="HE1" s="2"/>
-      <c r="HF1" s="2"/>
-      <c r="HG1" s="2"/>
-      <c r="HH1" s="2"/>
-      <c r="HI1" s="2"/>
-      <c r="HJ1" s="2"/>
-      <c r="HK1" s="2"/>
-      <c r="HL1" s="2"/>
-      <c r="HM1" s="2"/>
-      <c r="HN1" s="2"/>
-      <c r="HO1" s="2"/>
-      <c r="HP1" s="2"/>
-      <c r="HQ1" s="2"/>
-      <c r="HR1" s="2"/>
-      <c r="HS1" s="2"/>
-      <c r="HT1" s="3" t="s">
+      <c r="HE1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="HF1" s="3"/>
+      <c r="HG1" s="3"/>
+      <c r="HH1" s="3"/>
+      <c r="HI1" s="3"/>
+      <c r="HJ1" s="3"/>
+      <c r="HK1" s="3"/>
+      <c r="HL1" s="3"/>
+      <c r="HM1" s="3"/>
+      <c r="HN1" s="3"/>
+      <c r="HO1" s="3"/>
+      <c r="HP1" s="3"/>
+      <c r="HQ1" s="3"/>
+      <c r="HR1" s="3"/>
+      <c r="HS1" s="3"/>
+      <c r="HT1" s="3"/>
       <c r="HU1" s="3"/>
       <c r="HV1" s="3"/>
       <c r="HW1" s="3"/>
       <c r="HX1" s="3"/>
       <c r="HY1" s="3"/>
-      <c r="HZ1" s="3"/>
-      <c r="IA1" s="3"/>
-      <c r="IB1" s="3"/>
-      <c r="IC1" s="3"/>
-      <c r="ID1" s="3"/>
-      <c r="IE1" s="3"/>
-      <c r="IF1" s="3"/>
-      <c r="IG1" s="3"/>
-      <c r="IH1" s="3"/>
-      <c r="II1" s="3"/>
-      <c r="IJ1" s="3"/>
-      <c r="IK1" s="3"/>
-      <c r="IL1" s="3"/>
-      <c r="IM1" s="3"/>
-      <c r="IN1" s="3"/>
-      <c r="IO1" s="4" t="s">
+      <c r="HZ1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="IP1" s="4"/>
+      <c r="IA1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
@@ -1906,536 +1868,491 @@
       <c r="CD2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="CE2" s="16" t="s">
+      <c r="CE2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="CF2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="CG2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="CH2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="CI2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="CJ2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="CK2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="CL2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="CM2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="CN2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="CO2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="CP2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="CQ2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="CR2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="CS2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="CT2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="CU2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="CV2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="CW2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="CF2" s="16" t="s">
+      <c r="CX2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="CG2" s="16" t="s">
+      <c r="CY2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="CH2" s="16" t="s">
+      <c r="DA2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="CI2" s="16" t="s">
+      <c r="DB2" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="CJ2" s="16" t="s">
+      <c r="DC2" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="CK2" s="16" t="s">
+      <c r="DD2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="DE2" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="DF2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="DG2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="DH2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="DI2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="CL2" s="16" t="s">
+      <c r="DJ2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="CM2" s="16" t="s">
+      <c r="DK2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="CN2" s="16" t="s">
+      <c r="DL2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="CO2" s="16" t="s">
+      <c r="DM2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="CP2" s="16" t="s">
+      <c r="DN2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="CQ2" s="17" t="s">
+      <c r="DO2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="DP2" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="DQ2" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="DR2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CR2" s="17" t="s">
+      <c r="DS2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CS2" s="17" t="s">
+      <c r="DT2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="CT2" s="17" t="s">
+      <c r="DU2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="CU2" s="17" t="s">
+      <c r="DV2" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="CV2" s="17" t="s">
+      <c r="DW2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="CW2" s="17" t="s">
+      <c r="DX2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="CX2" s="17" t="s">
+      <c r="DY2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="CY2" s="17" t="s">
+      <c r="DZ2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="CZ2" s="17" t="s">
+      <c r="EA2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="DA2" s="17" t="s">
+      <c r="EB2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="DB2" s="17" t="s">
+      <c r="EC2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="DC2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="DD2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="DE2" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="DF2" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="DG2" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="DH2" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="DI2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="DJ2" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="DK2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="DM2" s="17" t="s">
+      <c r="ED2" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="DN2" s="17" t="s">
+      <c r="EE2" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="DO2" s="17" t="s">
+      <c r="EF2" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="DP2" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="DQ2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="DR2" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="DS2" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="DT2" s="17" t="s">
+      <c r="EG2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="EH2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="EI2" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="EJ2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="EK2" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="EL2" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="EM2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="EN2" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="EO2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="EP2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="EQ2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="ER2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="ES2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="ET2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="EU2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="EV2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="EW2" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="EX2" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="EY2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="EZ2" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="FA2" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="FB2" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="FC2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="FD2" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="FE2" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="FF2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="FG2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="FH2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="DU2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="DV2" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="DW2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="DX2" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="DY2" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="DZ2" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="EA2" s="17" t="s">
+      <c r="FI2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="FJ2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="FK2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="FL2" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="FM2" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="FN2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="FO2" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="FP2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="FQ2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="FR2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="FS2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="FT2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="FU2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="FV2" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="FW2" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="FX2" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="FY2" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="FZ2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="GA2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="GB2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="GC2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="GD2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="GE2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="GF2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="GG2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="GH2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="GI2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="GJ2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="GK2" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="GL2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="GM2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="GN2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="GO2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="GP2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="GQ2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="GR2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="GS2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="GT2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="GU2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="GV2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="EB2" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="EC2" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="ED2" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="EE2" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="EF2" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="EG2" s="18" t="s">
+      <c r="GW2" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="GX2" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="GY2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="GZ2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="HA2" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="HB2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="HC2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="HD2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="HE2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="EH2" s="18" t="s">
+      <c r="HF2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="EI2" s="18" t="s">
+      <c r="HG2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="EJ2" s="18" t="s">
+      <c r="HH2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="HI2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="EK2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="EL2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="EM2" s="18" t="s">
+      <c r="HJ2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="EN2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="EO2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="EP2" s="18" t="s">
+      <c r="HK2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="EQ2" s="18" t="s">
+      <c r="HL2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="ER2" s="18" t="s">
+      <c r="HM2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="ES2" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="ET2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="EU2" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="EV2" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="EW2" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="EX2" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="EY2" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="EZ2" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="FA2" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="FB2" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="FC2" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="FD2" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="FE2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="FF2" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="FG2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="FH2" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="FI2" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="FJ2" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="FK2" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="FL2" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="FM2" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="FN2" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="FO2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="FP2" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="FQ2" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="FR2" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="FS2" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="FT2" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="FU2" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="FV2" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="FW2" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="FX2" s="19" t="s">
+      <c r="HN2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="HO2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="FY2" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="FZ2" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="GA2" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="GB2" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="GC2" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="GD2" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="GE2" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="GF2" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="GG2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="GH2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="GI2" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="GJ2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="GK2" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="GL2" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="GM2" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="GN2" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="GO2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="GP2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="GQ2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="GR2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="GS2" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="GT2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="GU2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="GV2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="GW2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="GX2" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="GY2" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="GZ2" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="HA2" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="HB2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="HC2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="HD2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="HE2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="HF2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="HG2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="HH2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="HI2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="HJ2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="HK2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="HL2" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="HM2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="HN2" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="HO2" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="HP2" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="HQ2" s="12" t="s">
+      <c r="HP2" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="HR2" s="12" t="s">
+      <c r="HQ2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="HS2" s="12" t="s">
-        <v>31</v>
+      <c r="HR2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="HS2" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="HT2" s="13" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="HU2" s="13" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="HV2" s="13" t="s">
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="HW2" s="13" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="HX2" s="13" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="HY2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="HZ2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="IA2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="IB2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="IC2" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="ID2" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="IE2" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="IF2" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="IG2" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="IH2" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="II2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="IJ2" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="IK2" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="IL2" s="13" t="s">
+      <c r="HZ2" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="IM2" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="IN2" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="IO2" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="IP2" s="14" t="s">
+      <c r="IA2" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F3" s="0" t="str">
         <f aca="false">CONCATENATE("SAU_",B3,"_",C3,"_",D3,"_C-",E3)</f>
         <v>SAU_GeSo_1_1_C-1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0.16</v>
@@ -2447,10 +2364,10 @@
         <v>0.16</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>90</v>
@@ -2465,10 +2382,10 @@
         <v>1</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T3" s="0" t="n">
         <v>532</v>
@@ -2489,22 +2406,22 @@
         <v>75</v>
       </c>
       <c r="Z3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC3" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AD3" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AE3" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>164</v>
       </c>
       <c r="AF3" s="0" t="n">
         <v>31</v>
@@ -2513,7 +2430,7 @@
         <v>61</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AI3" s="0" t="n">
         <v>32</v>
@@ -2522,7 +2439,7 @@
         <v>62</v>
       </c>
       <c r="AK3" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AL3" s="0" t="n">
         <v>180</v>
@@ -2531,34 +2448,34 @@
         <v>50</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AO3" s="0" t="n">
         <v>900</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AR3" s="0" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>25</v>
       </c>
       <c r="AT3" s="0" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AU3" s="0" t="n">
         <v>1.42</v>
       </c>
       <c r="AV3" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AW3" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AX3" s="0" t="n">
         <v>0.5</v>
@@ -2576,7 +2493,7 @@
         <v>10</v>
       </c>
       <c r="BC3" s="0" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="BD3" s="0" t="n">
         <v>10</v>
@@ -2585,7 +2502,7 @@
         <v>1.5</v>
       </c>
       <c r="BF3" s="0" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="BG3" s="0" t="n">
         <v>20</v>
@@ -2594,13 +2511,13 @@
         <v>1.5</v>
       </c>
       <c r="BI3" s="0" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="BJ3" s="0" t="n">
         <v>1.42</v>
       </c>
       <c r="BK3" s="0" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="BL3" s="0" t="n">
         <v>1.42</v>
@@ -2630,7 +2547,7 @@
         <v>1002</v>
       </c>
       <c r="BU3" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="BV3" s="0" t="n">
         <v>0.3</v>
@@ -2645,7 +2562,7 @@
         <v>30</v>
       </c>
       <c r="BZ3" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="CA3" s="0" t="n">
         <v>30</v>
@@ -2654,55 +2571,55 @@
         <v>120</v>
       </c>
       <c r="CC3" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="CD3" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CE3" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="CF3" s="0" t="n">
-        <v>5</v>
+        <v>164</v>
+      </c>
+      <c r="CF3" s="0" t="s">
+        <v>165</v>
       </c>
       <c r="CG3" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="CH3" s="0" t="n">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="CH3" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="CI3" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="CJ3" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="CK3" s="0" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="CJ3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="CK3" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="CL3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="CM3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="CN3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="CO3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="CP3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="CL3" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="CM3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="CN3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="CO3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="CP3" s="0" t="n">
-        <v>0.01</v>
-      </c>
       <c r="CQ3" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="CR3" s="0" t="s">
         <v>168</v>
       </c>
+      <c r="CR3" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="CS3" s="0" t="n">
-        <v>25</v>
+        <v>1.5</v>
       </c>
       <c r="CT3" s="0" t="s">
         <v>169</v>
@@ -2710,459 +2627,414 @@
       <c r="CU3" s="0" t="n">
         <v>1.42</v>
       </c>
-      <c r="CV3" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="CW3" s="0" t="s">
-        <v>166</v>
+      <c r="CV3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="CW3" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="CX3" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="CY3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="CZ3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="DA3" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="CY3" s="0" t="n">
+      <c r="DB3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="DC3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="CZ3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="DA3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="DB3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="DC3" s="0" t="s">
+      <c r="DD3" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="DD3" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="DE3" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="DF3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="DF3" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="DG3" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="DG3" s="0" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="DH3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="DI3" s="0" t="n">
-        <v>25</v>
+      <c r="DH3" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="DI3" s="0" t="s">
+        <v>174</v>
       </c>
       <c r="DJ3" s="0" t="n">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="DK3" s="0" t="n">
         <v>15</v>
       </c>
       <c r="DL3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="DM3" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="DN3" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="DO3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="DP3" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="DQ3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="DR3" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="DS3" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="DT3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="DU3" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="DV3" s="0" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="DW3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="DX3" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="DY3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="DZ3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="EA3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="EB3" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="DM3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="DN3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="DO3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="DP3" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="DQ3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="DR3" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="DS3" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="DT3" s="0" t="s">
+      <c r="EC3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="ED3" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="DU3" s="0" t="s">
+      <c r="EE3" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="EF3" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="EG3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="EH3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="EI3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="EJ3" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="EK3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="EL3" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="EM3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="EN3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="EO3" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="DV3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="DW3" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="DX3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="DY3" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="DZ3" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="EA3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="EB3" s="0" t="s">
+      <c r="EP3" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="EC3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="ED3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="EE3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="EF3" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="EG3" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="EH3" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="EI3" s="0" t="n">
+      <c r="EQ3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="EJ3" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="EK3" s="0" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="EL3" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="EM3" s="0" t="s">
+      <c r="ER3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="ES3" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="EN3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="EO3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="EP3" s="0" t="n">
+      <c r="ET3" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="EU3" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="EQ3" s="0" t="n">
+      <c r="EV3" s="0" t="n">
         <v>45</v>
-      </c>
-      <c r="ER3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="ES3" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="ET3" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="EU3" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="EV3" s="0" t="n">
-        <v>3</v>
       </c>
       <c r="EW3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="EX3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="EY3" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="EZ3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="FA3" s="0" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="FB3" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="FC3" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="FD3" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="FE3" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="FF3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="FG3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="FH3" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="FI3" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="FJ3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="FK3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="FL3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="FM3" s="21" t="b">
+      <c r="EX3" s="21" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="FN3" s="0" t="n">
+      <c r="EY3" s="0" t="n">
         <v>1E-006</v>
       </c>
+      <c r="EZ3" s="0" t="n">
+        <v>5E-006</v>
+      </c>
+      <c r="FA3" s="0" t="n">
+        <v>3E-006</v>
+      </c>
+      <c r="FB3" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="FC3" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="FD3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="FE3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="FF3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FG3" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="FH3" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="FI3" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="FJ3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="FK3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="FL3" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="FM3" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="FN3" s="22" t="s">
+        <v>178</v>
+      </c>
       <c r="FO3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="FP3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="FQ3" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="FR3" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="FS3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="FT3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="FU3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="FV3" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="FW3" s="0" t="n">
         <v>5E-006</v>
       </c>
-      <c r="FP3" s="0" t="n">
+      <c r="FX3" s="0" t="n">
         <v>3E-006</v>
       </c>
-      <c r="FQ3" s="0" t="n">
+      <c r="FY3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="FZ3" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="GA3" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="GB3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="GC3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="GD3" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="GE3" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="GF3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="GG3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="GH3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="GI3" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="GJ3" s="0" t="n">
+        <v>5E-006</v>
+      </c>
+      <c r="GK3" s="0" t="n">
+        <v>3E-006</v>
+      </c>
+      <c r="GL3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="GM3" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="GN3" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="GO3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="GP3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="GQ3" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="GR3" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="GS3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="GT3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="GU3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="GV3" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="GW3" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="GX3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="GY3" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="GZ3" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="HA3" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="FR3" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="FS3" s="0" t="n">
+      <c r="HB3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="HC3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="HD3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="HE3" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="HF3" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="HG3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="FT3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="FU3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FV3" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="FW3" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="FX3" s="22" t="s">
+      <c r="HH3" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="HI3" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="HJ3" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="HK3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="HL3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="HM3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="HN3" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="FY3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="FZ3" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="GA3" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="GB3" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="GC3" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="GD3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="GE3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="GF3" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="GG3" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="GH3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="GI3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="GJ3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="GK3" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="GL3" s="0" t="n">
-        <v>5E-006</v>
-      </c>
-      <c r="GM3" s="0" t="n">
-        <v>3E-006</v>
-      </c>
-      <c r="GN3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="GO3" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="GP3" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="GQ3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="GR3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="GS3" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="GT3" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="GU3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="GV3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="GW3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="GX3" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="GY3" s="0" t="n">
-        <v>5E-006</v>
-      </c>
-      <c r="GZ3" s="0" t="n">
-        <v>3E-006</v>
-      </c>
-      <c r="HA3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="HB3" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="HC3" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="HD3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="HE3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="HF3" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="HG3" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="HH3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="HI3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="HJ3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="HK3" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="HL3" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="HM3" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="HN3" s="0" t="n">
-        <v>300</v>
-      </c>
       <c r="HO3" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="HP3" s="0" t="n">
-        <v>150</v>
+        <v>0.1</v>
       </c>
       <c r="HQ3" s="0" t="n">
-        <v>30</v>
+        <v>1800</v>
       </c>
       <c r="HR3" s="0" t="n">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="HS3" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="HT3" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="HU3" s="22" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+      <c r="HT3" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="HU3" s="0" t="n">
+        <v>80</v>
       </c>
       <c r="HV3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="HW3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="HX3" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="HY3" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="HZ3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="IA3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="IB3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="IC3" s="22" t="s">
+      <c r="HW3" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="HX3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="HY3" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="HZ3" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="IA3" s="22" t="s">
         <v>186</v>
-      </c>
-      <c r="ID3" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="IE3" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="IF3" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="IG3" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="IH3" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="II3" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="IJ3" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="IK3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="IL3" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="IM3" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="IN3" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="IO3" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="IP3" s="22" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3172,15 +3044,15 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AN1"/>
     <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:CP1"/>
-    <mergeCell ref="CQ1:EF1"/>
-    <mergeCell ref="EG1:FC1"/>
-    <mergeCell ref="FD1:GA1"/>
-    <mergeCell ref="GB1:GN1"/>
-    <mergeCell ref="GO1:HA1"/>
-    <mergeCell ref="HB1:HS1"/>
-    <mergeCell ref="HT1:IN1"/>
-    <mergeCell ref="IO1:IP1"/>
+    <mergeCell ref="AQ1:CD1"/>
+    <mergeCell ref="CE1:DQ1"/>
+    <mergeCell ref="DR1:EN1"/>
+    <mergeCell ref="EO1:FL1"/>
+    <mergeCell ref="FM1:FY1"/>
+    <mergeCell ref="FZ1:GL1"/>
+    <mergeCell ref="GM1:HD1"/>
+    <mergeCell ref="HE1:HY1"/>
+    <mergeCell ref="HZ1:IA1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>